<commit_message>
Updating plots and code
</commit_message>
<xml_diff>
--- a/CCK8_Assay_Plots/20231006_PolymerScreening_AW copy.xlsx
+++ b/CCK8_Assay_Plots/20231006_PolymerScreening_AW copy.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mines0-my.sharepoint.com/personal/aryellewright_mines_edu/Documents/Research/Kumar Research Lab/Aryelle's Lab Notebook/CCK8 Plate Reader Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aryellewright/Documents/Kumar-Biomaterials-Lab/CCK8_Assay_Plots/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="149" documentId="11_9F98414E98627E7275D89F1FA240F7EC1F97DA51" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4B96A4E4-530E-1D4D-90A0-850489173C66}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68104614-6627-B147-B91D-A9E7E2EFFDFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17340" yWindow="1100" windowWidth="18040" windowHeight="18140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13000" yWindow="640" windowWidth="12600" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plate 1 - Sheet1" sheetId="1" r:id="rId1"/>
@@ -658,6 +658,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -667,7 +668,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -685,8 +685,97 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>10143</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>145155</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D9D3CDB-0509-F2E7-CD30-5D1F0EF1EDE9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8648700" y="340343"/>
+          <a:ext cx="5232400" cy="3792612"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>111743</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>600545</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{331CED36-20A1-B731-10A8-69CBDFFF4CAE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10998200" y="4264643"/>
+          <a:ext cx="4296245" cy="3114057"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -954,7 +1043,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:O67"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E30" workbookViewId="0">
       <selection activeCell="D40" sqref="D40:I55"/>
     </sheetView>
   </sheetViews>
@@ -1196,7 +1285,7 @@
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="B36" s="52" t="s">
+      <c r="B36" s="53" t="s">
         <v>32</v>
       </c>
       <c r="C36" s="7"/>
@@ -1216,7 +1305,7 @@
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="B37" s="53"/>
+      <c r="B37" s="54"/>
       <c r="C37" s="9"/>
       <c r="D37" s="9"/>
       <c r="E37" s="9"/>
@@ -1234,7 +1323,7 @@
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="B38" s="53"/>
+      <c r="B38" s="54"/>
       <c r="C38" s="9"/>
       <c r="D38" s="9"/>
       <c r="E38" s="9"/>
@@ -1252,7 +1341,7 @@
       </c>
     </row>
     <row r="39" spans="1:15" ht="36" x14ac:dyDescent="0.15">
-      <c r="B39" s="54"/>
+      <c r="B39" s="55"/>
       <c r="C39" s="10"/>
       <c r="D39" s="10"/>
       <c r="E39" s="10"/>
@@ -1270,7 +1359,7 @@
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="B40" s="52" t="s">
+      <c r="B40" s="53" t="s">
         <v>37</v>
       </c>
       <c r="C40" s="7"/>
@@ -1302,7 +1391,7 @@
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="B41" s="53"/>
+      <c r="B41" s="54"/>
       <c r="C41" s="9"/>
       <c r="D41" s="15">
         <v>0.54</v>
@@ -1332,7 +1421,7 @@
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="B42" s="53"/>
+      <c r="B42" s="54"/>
       <c r="C42" s="9"/>
       <c r="D42" s="15">
         <v>3.9E-2</v>
@@ -1362,7 +1451,7 @@
       </c>
     </row>
     <row r="43" spans="1:15" ht="36" x14ac:dyDescent="0.15">
-      <c r="B43" s="54"/>
+      <c r="B43" s="55"/>
       <c r="C43" s="10"/>
       <c r="D43" s="24">
         <v>52398</v>
@@ -1392,7 +1481,7 @@
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="B44" s="52" t="s">
+      <c r="B44" s="53" t="s">
         <v>38</v>
       </c>
       <c r="C44" s="7"/>
@@ -1424,7 +1513,7 @@
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="B45" s="53"/>
+      <c r="B45" s="54"/>
       <c r="C45" s="9"/>
       <c r="D45" s="20">
         <v>0.156</v>
@@ -1454,7 +1543,7 @@
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="B46" s="53"/>
+      <c r="B46" s="54"/>
       <c r="C46" s="9"/>
       <c r="D46" s="15">
         <v>3.9E-2</v>
@@ -1484,7 +1573,7 @@
       </c>
     </row>
     <row r="47" spans="1:15" ht="36" x14ac:dyDescent="0.15">
-      <c r="B47" s="54"/>
+      <c r="B47" s="55"/>
       <c r="C47" s="10"/>
       <c r="D47" s="29">
         <v>1642429</v>
@@ -1514,7 +1603,7 @@
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="B48" s="52" t="s">
+      <c r="B48" s="53" t="s">
         <v>39</v>
       </c>
       <c r="C48" s="7"/>
@@ -1546,7 +1635,7 @@
       </c>
     </row>
     <row r="49" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B49" s="53"/>
+      <c r="B49" s="54"/>
       <c r="C49" s="9"/>
       <c r="D49" s="35">
         <v>0.504</v>
@@ -1576,7 +1665,7 @@
       </c>
     </row>
     <row r="50" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B50" s="53"/>
+      <c r="B50" s="54"/>
       <c r="C50" s="9"/>
       <c r="D50" s="20">
         <v>3.6999999999999998E-2</v>
@@ -1606,7 +1695,7 @@
       </c>
     </row>
     <row r="51" spans="2:15" ht="36" x14ac:dyDescent="0.15">
-      <c r="B51" s="54"/>
+      <c r="B51" s="55"/>
       <c r="C51" s="10"/>
       <c r="D51" s="24">
         <v>54573</v>
@@ -1636,7 +1725,7 @@
       </c>
     </row>
     <row r="52" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B52" s="52" t="s">
+      <c r="B52" s="53" t="s">
         <v>40</v>
       </c>
       <c r="C52" s="7"/>
@@ -1668,7 +1757,7 @@
       </c>
     </row>
     <row r="53" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B53" s="53"/>
+      <c r="B53" s="54"/>
       <c r="C53" s="9"/>
       <c r="D53" s="27">
         <v>0.21299999999999999</v>
@@ -1698,7 +1787,7 @@
       </c>
     </row>
     <row r="54" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B54" s="53"/>
+      <c r="B54" s="54"/>
       <c r="C54" s="9"/>
       <c r="D54" s="27">
         <v>3.6999999999999998E-2</v>
@@ -1728,7 +1817,7 @@
       </c>
     </row>
     <row r="55" spans="2:15" ht="36" x14ac:dyDescent="0.15">
-      <c r="B55" s="54"/>
+      <c r="B55" s="55"/>
       <c r="C55" s="10"/>
       <c r="D55" s="38">
         <v>453598</v>
@@ -1758,7 +1847,7 @@
       </c>
     </row>
     <row r="56" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B56" s="52" t="s">
+      <c r="B56" s="53" t="s">
         <v>41</v>
       </c>
       <c r="C56" s="7"/>
@@ -1778,7 +1867,7 @@
       </c>
     </row>
     <row r="57" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B57" s="53"/>
+      <c r="B57" s="54"/>
       <c r="C57" s="9"/>
       <c r="D57" s="9"/>
       <c r="E57" s="9"/>
@@ -1796,7 +1885,7 @@
       </c>
     </row>
     <row r="58" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B58" s="53"/>
+      <c r="B58" s="54"/>
       <c r="C58" s="9"/>
       <c r="D58" s="9"/>
       <c r="E58" s="9"/>
@@ -1814,7 +1903,7 @@
       </c>
     </row>
     <row r="59" spans="2:15" ht="36" x14ac:dyDescent="0.15">
-      <c r="B59" s="54"/>
+      <c r="B59" s="55"/>
       <c r="C59" s="10"/>
       <c r="D59" s="10"/>
       <c r="E59" s="10"/>
@@ -1832,7 +1921,7 @@
       </c>
     </row>
     <row r="60" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B60" s="52" t="s">
+      <c r="B60" s="53" t="s">
         <v>42</v>
       </c>
       <c r="C60" s="7"/>
@@ -1852,7 +1941,7 @@
       </c>
     </row>
     <row r="61" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B61" s="53"/>
+      <c r="B61" s="54"/>
       <c r="C61" s="9"/>
       <c r="D61" s="9"/>
       <c r="E61" s="9"/>
@@ -1870,7 +1959,7 @@
       </c>
     </row>
     <row r="62" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B62" s="53"/>
+      <c r="B62" s="54"/>
       <c r="C62" s="9"/>
       <c r="D62" s="9"/>
       <c r="E62" s="9"/>
@@ -1888,7 +1977,7 @@
       </c>
     </row>
     <row r="63" spans="2:15" ht="36" x14ac:dyDescent="0.15">
-      <c r="B63" s="54"/>
+      <c r="B63" s="55"/>
       <c r="C63" s="10"/>
       <c r="D63" s="10"/>
       <c r="E63" s="10"/>
@@ -1906,7 +1995,7 @@
       </c>
     </row>
     <row r="64" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B64" s="52" t="s">
+      <c r="B64" s="53" t="s">
         <v>43</v>
       </c>
       <c r="C64" s="7"/>
@@ -1926,7 +2015,7 @@
       </c>
     </row>
     <row r="65" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B65" s="53"/>
+      <c r="B65" s="54"/>
       <c r="C65" s="9"/>
       <c r="D65" s="9"/>
       <c r="E65" s="9"/>
@@ -1944,7 +2033,7 @@
       </c>
     </row>
     <row r="66" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B66" s="53"/>
+      <c r="B66" s="54"/>
       <c r="C66" s="9"/>
       <c r="D66" s="9"/>
       <c r="E66" s="9"/>
@@ -1962,7 +2051,7 @@
       </c>
     </row>
     <row r="67" spans="2:15" ht="36" x14ac:dyDescent="0.15">
-      <c r="B67" s="54"/>
+      <c r="B67" s="55"/>
       <c r="C67" s="10"/>
       <c r="D67" s="10"/>
       <c r="E67" s="10"/>
@@ -2000,8 +2089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AC5F8D7-B342-8848-AC05-5066C16FEDF1}">
   <dimension ref="A1:S56"/>
   <sheetViews>
-    <sheetView topLeftCell="E16" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27:M35"/>
+    <sheetView topLeftCell="L8" workbookViewId="0">
+      <selection activeCell="N44" sqref="N44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2938,6 +3027,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2945,8 +3035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9E70CCE-BE82-AF4E-AA5A-8622B4ADB83C}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3020,11 +3110,11 @@
         <v>4.1952719131609051</v>
       </c>
       <c r="D3" s="44">
-        <f t="shared" ref="D3:D8" si="0">AVERAGE(F3:H3)</f>
+        <f t="shared" ref="D3:D4" si="0">AVERAGE(F3:H3)</f>
         <v>3.6666666666666674E-2</v>
       </c>
       <c r="E3" s="44">
-        <f t="shared" ref="E3:E8" si="1">STDEV(F3:H3,D3)</f>
+        <f t="shared" ref="E3:E5" si="1">STDEV(F3:H3,D3)</f>
         <v>1.2472191289246457E-2</v>
       </c>
       <c r="F3" s="44">
@@ -3189,10 +3279,10 @@
         <f t="shared" si="3"/>
         <v>0.65999999999999925</v>
       </c>
-      <c r="F9" s="55">
+      <c r="F9" s="52">
         <v>14.74</v>
       </c>
-      <c r="G9" s="55">
+      <c r="G9" s="52">
         <v>16.059999999999999</v>
       </c>
     </row>
@@ -3214,10 +3304,10 @@
         <f t="shared" si="3"/>
         <v>0.15500000000000005</v>
       </c>
-      <c r="F10" s="55">
+      <c r="F10" s="52">
         <v>0.27</v>
       </c>
-      <c r="G10" s="55">
+      <c r="G10" s="52">
         <v>0.57999999999999996</v>
       </c>
     </row>

</xml_diff>